<commit_message>
Files feature working. can save files to the server.
</commit_message>
<xml_diff>
--- a/Docs/Communication Protocol.xlsx
+++ b/Docs/Communication Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avrah\Desktop\personal\CodeProjects\mechineLearinig\Mousey3.0\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA001FE2-02F1-453F-AAA8-CCB9E3B7B177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6054912-E063-44CE-AA1F-85DA94F7075B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAFE5224-59CD-4F41-8567-09308282B003}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>opcode</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>{speed:value}</t>
+  </si>
+  <si>
+    <t>name - 40</t>
+  </si>
+  <si>
+    <t>date - 10</t>
+  </si>
+  <si>
+    <t>fileSize - 15</t>
+  </si>
+  <si>
+    <t>data Size - 20</t>
+  </si>
+  <si>
+    <t>data - all the rest</t>
   </si>
 </sst>
 </file>
@@ -177,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,31 +320,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -640,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9BC892-70DF-449E-B611-2720F9D3DCE1}">
-  <dimension ref="B2:H28"/>
+  <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -655,22 +682,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -713,19 +740,19 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="18">
         <v>20</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -733,31 +760,31 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
@@ -783,19 +810,19 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="10">
         <v>22</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -803,39 +830,39 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>23</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -843,29 +870,29 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="10">
         <v>24</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -873,29 +900,29 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>25</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -903,39 +930,39 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="10">
         <v>26</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -943,11 +970,11 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
@@ -956,117 +983,162 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="19">
         <v>27</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="18">
         <v>28</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C29" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D29" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E29" s="13">
         <v>29</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="1" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="1" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E32" s="5">
         <v>30</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
+  <mergeCells count="41">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="F29:F31"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
@@ -1077,18 +1149,20 @@
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finish writing the logout protocol msg the same as the end of the three hand shake of the tcp protocol just in udp and for mousey only. Changed some of the UI client side and Server Side.
</commit_message>
<xml_diff>
--- a/Docs/Communication Protocol.xlsx
+++ b/Docs/Communication Protocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avrah\Desktop\personal\CodeProjects\mechineLearinig\Mousey3.0\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6054912-E063-44CE-AA1F-85DA94F7075B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC97D7B-006E-4991-ABA6-3D81F6ED8C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAFE5224-59CD-4F41-8567-09308282B003}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>opcode</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>data - all the rest</t>
+  </si>
+  <si>
+    <t>Client / Server</t>
+  </si>
+  <si>
+    <t>Server / Client</t>
+  </si>
+  <si>
+    <t>Ack Logout Mousey</t>
+  </si>
+  <si>
+    <t>FIN</t>
   </si>
 </sst>
 </file>
@@ -192,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,12 +232,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,12 +332,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,17 +356,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9BC892-70DF-449E-B611-2720F9D3DCE1}">
-  <dimension ref="B2:H32"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -682,22 +697,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -740,19 +755,19 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="13">
         <v>20</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -760,31 +775,31 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
@@ -830,39 +845,39 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="14">
         <v>23</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -870,11 +885,11 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
@@ -900,29 +915,29 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
       <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="14">
         <v>25</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="14" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -930,21 +945,21 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="7" t="s">
         <v>22</v>
       </c>
@@ -970,11 +985,11 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
@@ -982,15 +997,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="28" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>7</v>
+      <c r="C23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="E23" s="19">
         <v>27</v>
@@ -998,22 +1013,24 @@
       <c r="F23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="21" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="13">
         <v>28</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G24" s="9" t="s">
@@ -1021,59 +1038,59 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="16">
         <v>29</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -1081,21 +1098,21 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
       <c r="G30" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
       <c r="G31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1120,24 +1137,53 @@
         <v>37</v>
       </c>
     </row>
+    <row r="33" spans="2:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="19">
+        <v>31</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="22">
+        <v>32</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="F29:F31"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -1150,17 +1196,28 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="F24:F28"/>
-    <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="E18:E20"/>
   </mergeCells>

</xml_diff>

<commit_message>
added new feature after sending a file to mousey we can save the file where we want and open it after we double click on his name
</commit_message>
<xml_diff>
--- a/Docs/Communication Protocol.xlsx
+++ b/Docs/Communication Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avrah\Desktop\personal\CodeProjects\mechineLearinig\Mousey3.0\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC97D7B-006E-4991-ABA6-3D81F6ED8C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81812CD2-1A42-4DAA-A144-300591DBF137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAFE5224-59CD-4F41-8567-09308282B003}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>opcode</t>
   </si>
@@ -180,13 +180,22 @@
   </si>
   <si>
     <t>FIN</t>
+  </si>
+  <si>
+    <t>Mousey Battery</t>
+  </si>
+  <si>
+    <t>Mousey Start Veiwer</t>
+  </si>
+  <si>
+    <t>Mousey Veiwer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +210,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -300,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -329,33 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +357,57 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,37 +723,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9BC892-70DF-449E-B611-2720F9D3DCE1}">
-  <dimension ref="B2:H34"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B37" sqref="B36:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.25" customWidth="1"/>
     <col min="3" max="4" width="8.9140625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.08203125" customWidth="1"/>
     <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -755,19 +796,19 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="21">
         <v>20</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -775,31 +816,31 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
@@ -825,19 +866,19 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="17">
         <v>22</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -845,39 +886,39 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="20">
         <v>23</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -885,29 +926,29 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="17">
         <v>24</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -915,29 +956,29 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="B18" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="20">
         <v>25</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="20" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -945,39 +986,39 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="B21" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="17">
         <v>26</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="17" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -985,11 +1026,11 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
@@ -998,39 +1039,39 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="28" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="20" t="s">
+      <c r="B23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="10">
         <v>27</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="21">
         <v>28</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G24" s="9" t="s">
@@ -1038,59 +1079,59 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="14">
         <v>29</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -1098,21 +1139,21 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1138,52 +1179,141 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="20" t="s">
+      <c r="B33" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="10">
         <v>31</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="22" t="s">
+      <c r="B34" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="13">
         <v>32</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="13" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="10">
+        <v>33</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="23">
+        <v>34</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="25">
+        <v>35</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="28"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G39" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B21:B22"/>
+  <mergeCells count="46">
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F29:F31"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -1200,28 +1330,17 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="D24:D28"/>
     <mergeCell ref="E24:E28"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished the viewer feature including zoom in and zoom out
</commit_message>
<xml_diff>
--- a/Docs/Communication Protocol.xlsx
+++ b/Docs/Communication Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avrah\Desktop\personal\CodeProjects\mechineLearinig\Mousey3.0\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81812CD2-1A42-4DAA-A144-300591DBF137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E14E71D-EF6C-4A5A-89D3-DFC6A0B12F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CAFE5224-59CD-4F41-8567-09308282B003}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
   <si>
     <t>opcode</t>
   </si>
@@ -185,10 +185,22 @@
     <t>Mousey Battery</t>
   </si>
   <si>
-    <t>Mousey Start Veiwer</t>
-  </si>
-  <si>
     <t>Mousey Veiwer</t>
+  </si>
+  <si>
+    <t>Mousey Start Viewer</t>
+  </si>
+  <si>
+    <t>Mousey End Viewer</t>
+  </si>
+  <si>
+    <t>Ack End Viewer</t>
+  </si>
+  <si>
+    <t>Viewer Zoom</t>
+  </si>
+  <si>
+    <t>state: in \ out - 10</t>
   </si>
 </sst>
 </file>
@@ -214,7 +226,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
@@ -317,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,9 +345,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -358,31 +366,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,6 +407,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9BC892-70DF-449E-B611-2720F9D3DCE1}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B37" sqref="B36:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -738,22 +764,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -796,19 +822,19 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="17">
         <v>20</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -816,31 +842,31 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
@@ -866,19 +892,19 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="13">
         <v>22</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -886,39 +912,39 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="B14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="15">
         <v>23</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -926,29 +952,29 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>24</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -956,69 +982,69 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="20" t="s">
+      <c r="B18" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="15">
         <v>25</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="7" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="13">
         <v>26</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -1026,11 +1052,11 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1039,269 +1065,341 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="28" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>27</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="17">
         <v>28</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="9" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="9" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="9" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="27">
+        <v>29</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="19">
+        <v>30</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="B34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="9">
+        <v>31</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="B35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="12">
+        <v>32</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="14">
-        <v>29</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="E36" s="9">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="1" t="s">
+      <c r="F36" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="19">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="1" t="s">
+      <c r="F37" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="21">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="F38" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E40" s="19">
+        <v>36</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="5">
-        <v>30</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="E41" s="9">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="10">
-        <v>31</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="12" t="s">
+      <c r="F41" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="B34" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="13">
-        <v>32</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="11" t="s">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="10">
-        <v>33</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="23">
-        <v>34</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="25">
-        <v>35</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G39" s="8"/>
+      <c r="E42" s="19">
+        <v>38</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C18:C20"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="F6:F9"/>
@@ -1314,31 +1412,26 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F29:F31"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F29:F32"/>
     <mergeCell ref="F18:F20"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>